<commit_message>
alteração no módulo de gerar atas
</commit_message>
<xml_diff>
--- a/database/relatorio.xlsx
+++ b/database/relatorio.xlsx
@@ -665,8 +665,14 @@
       <c r="W2" t="n">
         <v>62.84549161758042</v>
       </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
+      <c r="X2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z2" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 7.000 a 10.000 btu´s.</t>
@@ -773,8 +779,14 @@
       <c r="W3" t="n">
         <v>42.06257242178447</v>
       </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+      <c r="X3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z3" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 12.000 a 18.000 btu´s.</t>
@@ -881,8 +893,14 @@
       <c r="W4" t="n">
         <v>84.94623655913979</v>
       </c>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="X4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z4" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 22.000 a 24.000 btu´s.</t>
@@ -989,8 +1007,14 @@
       <c r="W5" t="n">
         <v>30.00069478218579</v>
       </c>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
+      <c r="X5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z5" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 30.000 a 36.000 btu´s.</t>
@@ -1097,8 +1121,14 @@
       <c r="W6" t="n">
         <v>56.89159673525693</v>
       </c>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
+      <c r="X6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z6" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 42.000 a 60.000 btu´s.</t>
@@ -1205,8 +1235,14 @@
       <c r="W7" t="n">
         <v>76.01106313323737</v>
       </c>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
+      <c r="X7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z7" t="inlineStr">
         <is>
           <t>Serviço de manutençao corretiva com fornecimento e substituição de motoventilador da evaporadora de condicionador de ar tipo split de 7.000 a 10.000 btu´s, de todos os modelos da marca springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -1313,8 +1349,14 @@
       <c r="W8" t="n">
         <v>70.81712062256808</v>
       </c>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
+      <c r="X8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z8" t="inlineStr">
         <is>
           <t>Serviço de manutençao corretiva com fornecimento e substituição de motoventilador da evaporadora de condicionador de ar tipo split de 12.000 a 18.000 btu´s, de todos os modelos da marca springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -1421,8 +1463,14 @@
       <c r="W9" t="n">
         <v>51.81989400376681</v>
       </c>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
+      <c r="X9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z9" t="inlineStr">
         <is>
           <t>Serviço de manutençao corretiva com fornecimento e substituição de motoventilador da evaporadora de condicionador de ar tipo split de 22.000 a 24.000 btu´s, de todos os modelos da marca springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -1529,8 +1577,14 @@
       <c r="W10" t="n">
         <v>78.18229901269393</v>
       </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
+      <c r="X10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z10" t="inlineStr">
         <is>
           <t>Serviço de manutençao corretiva com fornecimento e substituição de motoventilador da evaporadora de condicionador de ar tipo split de 30.000 a 36.000 btu´s, de todos os modelos da marca springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -1637,8 +1691,14 @@
       <c r="W11" t="n">
         <v>86.84441326083143</v>
       </c>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
+      <c r="X11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z11" t="inlineStr">
         <is>
           <t>Serviço de manutençao corretiva com fornecimento e substituição de motoventilador da evaporadora de condicionador de ar tipo split de 42.000 a 60.000 btu´s, de todos os modelos da marca springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -1745,8 +1805,14 @@
       <c r="W12" t="n">
         <v>81.20228641577474</v>
       </c>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
+      <c r="X12" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z12" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de motoventilador da condensadora de condicionador de ar tipo split de 7.000 a 10.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -1853,8 +1919,14 @@
       <c r="W13" t="n">
         <v>54.6163105033643</v>
       </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
+      <c r="X13" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z13" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de motoventilador da condensadora de condicionador de ar tipo split de 12.000 a 18.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -1961,8 +2033,14 @@
       <c r="W14" t="n">
         <v>53.98490704951224</v>
       </c>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
+      <c r="X14" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z14" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de motoventilador da condensadora de condicionador de ar tipo split de 22.000 a 24.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, 50york, consul, lg, gree e eletrolux e komeco.</t>
@@ -2069,8 +2147,14 @@
       <c r="W15" t="n">
         <v>53.88871810636336</v>
       </c>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
+      <c r="X15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z15" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de motoventilador da condensadora de condicionador de ar tipo split de 30.000 a 36.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -2177,8 +2261,14 @@
       <c r="W16" t="n">
         <v>64.4781244449707</v>
       </c>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
+      <c r="X16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z16" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de motoventilador da condensadora de condicionador de ar tipo split de 42.000 a 60.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -2285,8 +2375,14 @@
       <c r="W17" t="n">
         <v>83.54680828907632</v>
       </c>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
+      <c r="X17" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z17" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva de substituição de compressor rotativo convencional/inverter com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 7.000 a 10.000 btu´s.</t>
@@ -2393,8 +2489,14 @@
       <c r="W18" t="n">
         <v>30.00258531540848</v>
       </c>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
+      <c r="X18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z18" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva de substituição de compressor rotativo convencional/inverter com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 12.000 a 18.000 btu´s.</t>
@@ -2501,8 +2603,14 @@
       <c r="W19" t="n">
         <v>30.00111232937661</v>
       </c>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
+      <c r="X19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z19" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva de substituição de compressor rotativo convencional/inverter com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 22.000 a 24.000 btu´s.</t>
@@ -2609,8 +2717,14 @@
       <c r="W20" t="n">
         <v>30.00031098878886</v>
       </c>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
+      <c r="X20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z20" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva de substituição de compressor rotativo convencional/inverter com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 30.000 a 36.000 btu´s.</t>
@@ -2717,8 +2831,14 @@
       <c r="W21" t="n">
         <v>29.97773930249814</v>
       </c>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
+      <c r="X21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z21" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva de substituição de compressor rotativo convencional/inverter com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 42.000 a 60.000 btu´s.</t>
@@ -2825,8 +2945,14 @@
       <c r="W22" t="n">
         <v>30.00273124544792</v>
       </c>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
+      <c r="X22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z22" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com retirada de vazamento (serviço de solda), fornecimento e carga de gás r-22 ou r-410a de condicionador de ar split ou janela de 7.000 a 10.000 btu´s.</t>
@@ -2933,8 +3059,14 @@
       <c r="W23" t="n">
         <v>69.20742591931453</v>
       </c>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
+      <c r="X23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z23" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com retirada de vazamento (serviço de solda), fornecimento e carga de gás r-22 ou r-410a de condicionador de ar split ou janela de 12.000 a 18.000 btu´s.</t>
@@ -3041,8 +3173,14 @@
       <c r="W24" t="n">
         <v>56.41931684334511</v>
       </c>
-      <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="inlineStr"/>
+      <c r="X24" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z24" t="inlineStr">
         <is>
           <t>Serviço de manuteção corretiva com retirada de vazamento (serviço de solda), fornecimento e carga de gás r-22 ou r-410a de condicionador de ar split ou janela de 22.000 a 24.000 btu´s.</t>
@@ -3149,8 +3287,14 @@
       <c r="W25" t="n">
         <v>31.11405789863433</v>
       </c>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
+      <c r="X25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z25" t="inlineStr">
         <is>
           <t>Serviço de manuteção corretiva com retirada de vazamento (serviço de solda), fornecimento e carga de gás r-22 ou r-410a de condicionador de ar split ou janela de 30.000 a 36.000 btu´s.</t>
@@ -3257,8 +3401,14 @@
       <c r="W26" t="n">
         <v>85.0831193196672</v>
       </c>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr"/>
+      <c r="X26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z26" t="inlineStr">
         <is>
           <t>Serviço de manuteção corretiva com retirada de vazamento (serviço de solda), fornecimento e carga de gás r-22 ou r-410a de condicionador de ar split ou janela de 42.000 a 60.000 btu´s.</t>
@@ -3365,8 +3515,14 @@
       <c r="W27" t="n">
         <v>2.251584198462997</v>
       </c>
-      <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
+      <c r="X27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z27" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 7.000 a 10.000 btu´s.</t>
@@ -3473,8 +3629,14 @@
       <c r="W28" t="n">
         <v>59.39731924469229</v>
       </c>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
+      <c r="X28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z28" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 12.000 a 18.000 btu´s.</t>
@@ -3581,8 +3743,14 @@
       <c r="W29" t="n">
         <v>3.684770661409353</v>
       </c>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="inlineStr"/>
+      <c r="X29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z29" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 22.000 a 24.000 btu´s.</t>
@@ -3689,8 +3857,14 @@
       <c r="W30" t="n">
         <v>65.76339079377578</v>
       </c>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
+      <c r="X30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z30" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 30.000 a 36.000 btu´s.</t>
@@ -3797,8 +3971,14 @@
       <c r="W31" t="n">
         <v>62.18436839300754</v>
       </c>
-      <c r="X31" t="inlineStr"/>
-      <c r="Y31" t="inlineStr"/>
+      <c r="X31" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z31" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e carga de gás r-22 ou r-410a de condicionador de ar tipo split ou janela de 42.000 a 60.000 btu´s.</t>
@@ -3905,8 +4085,14 @@
       <c r="W32" t="n">
         <v>48.11957569913211</v>
       </c>
-      <c r="X32" t="inlineStr"/>
-      <c r="Y32" t="inlineStr"/>
+      <c r="X32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z32" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação de turbina da evaporadora de condicionador de ar tipo split 7.000 a 10.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4013,8 +4199,14 @@
       <c r="W33" t="n">
         <v>40.20789255818231</v>
       </c>
-      <c r="X33" t="inlineStr"/>
-      <c r="Y33" t="inlineStr"/>
+      <c r="X33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z33" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação de turbina da evaporadora de condicionador de ar tipo split 12.000 a 18.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4121,8 +4313,14 @@
       <c r="W34" t="n">
         <v>57.03592151304425</v>
       </c>
-      <c r="X34" t="inlineStr"/>
-      <c r="Y34" t="inlineStr"/>
+      <c r="X34" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z34" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação de turbina da evaporadora de condicionador de ar tipo split 22.000 a 24.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4229,8 +4427,14 @@
       <c r="W35" t="n">
         <v>30</v>
       </c>
-      <c r="X35" t="inlineStr"/>
-      <c r="Y35" t="inlineStr"/>
+      <c r="X35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z35" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação de turbina da evaporadora de condicionador de ar tipo split 30.000 a 36.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4337,8 +4541,14 @@
       <c r="W36" t="n">
         <v>60.48278397255238</v>
       </c>
-      <c r="X36" t="inlineStr"/>
-      <c r="Y36" t="inlineStr"/>
+      <c r="X36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z36" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação de turbina da evaporadora de condicionador de ar tipo split 42.000 a 60.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4445,8 +4655,14 @@
       <c r="W37" t="n">
         <v>30.00598324690866</v>
       </c>
-      <c r="X37" t="inlineStr"/>
-      <c r="Y37" t="inlineStr"/>
+      <c r="X37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z37" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação da hélice da condensadora de condicionador de ar tipo split 7.000 a 10.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4553,8 +4769,14 @@
       <c r="W38" t="n">
         <v>30.00083451556372</v>
       </c>
-      <c r="X38" t="inlineStr"/>
-      <c r="Y38" t="inlineStr"/>
+      <c r="X38" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z38" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação da hélice da condensadora de condicionador de ar tipo split 12.000 a 18.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4661,8 +4883,14 @@
       <c r="W39" t="n">
         <v>30.07124109486315</v>
       </c>
-      <c r="X39" t="inlineStr"/>
-      <c r="Y39" t="inlineStr"/>
+      <c r="X39" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z39" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação da hélice da condensadora de condicionador de ar tipo split 22.000 a 24.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4769,8 +4997,14 @@
       <c r="W40" t="n">
         <v>30.00194817845314</v>
       </c>
-      <c r="X40" t="inlineStr"/>
-      <c r="Y40" t="inlineStr"/>
+      <c r="X40" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z40" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação da hélice da condensadora de condicionador de ar tipo split 30.000 a 36.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4877,8 +5111,14 @@
       <c r="W41" t="n">
         <v>29.82386386227187</v>
       </c>
-      <c r="X41" t="inlineStr"/>
-      <c r="Y41" t="inlineStr"/>
+      <c r="X41" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z41" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e instalação da hélice da condensadora de condicionador de ar tipo split 42.000 a 60.000 btu´s. De todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -4985,8 +5225,14 @@
       <c r="W42" t="n">
         <v>27.40998838559814</v>
       </c>
-      <c r="X42" t="inlineStr"/>
-      <c r="Y42" t="inlineStr"/>
+      <c r="X42" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z42" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de sensor de degelo ou ambiente de condicionador de ar tipo split de 7.000 a 10.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5093,8 +5339,14 @@
       <c r="W43" t="n">
         <v>82.78829604130809</v>
       </c>
-      <c r="X43" t="inlineStr"/>
-      <c r="Y43" t="inlineStr"/>
+      <c r="X43" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z43" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de sensor de degelo ou ambiente de condicionador de ar tipo split de 12.000 a 18.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5201,8 +5453,14 @@
       <c r="W44" t="n">
         <v>60.3756970942178</v>
       </c>
-      <c r="X44" t="inlineStr"/>
-      <c r="Y44" t="inlineStr"/>
+      <c r="X44" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z44" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de sensor de degelo ou ambiente de condicionador de ar tipo split de 22.000 a 24.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5309,8 +5567,14 @@
       <c r="W45" t="n">
         <v>43.2986037281168</v>
       </c>
-      <c r="X45" t="inlineStr"/>
-      <c r="Y45" t="inlineStr"/>
+      <c r="X45" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z45" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de sensor de degelo ou ambiente de condicionador de ar tipo split de 30.000 a 36.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5417,8 +5681,14 @@
       <c r="W46" t="n">
         <v>10.66997518610422</v>
       </c>
-      <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr"/>
+      <c r="X46" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z46" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de sensor de degelo ou ambiente de condicionador de ar tipo split de 42.000 a 60.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5525,8 +5795,14 @@
       <c r="W47" t="n">
         <v>9.077132898924066</v>
       </c>
-      <c r="X47" t="inlineStr"/>
-      <c r="Y47" t="inlineStr"/>
+      <c r="X47" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z47" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento de placa receptora de condicionador de ar tipo split de 7.000 a 10.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5633,8 +5909,14 @@
       <c r="W48" t="n">
         <v>9.042674145380126</v>
       </c>
-      <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="inlineStr"/>
+      <c r="X48" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z48" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento de placa receptora de condicionador de ar tipo split de 12.000 a 18.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5739,8 +6021,14 @@
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
-      <c r="X49" t="inlineStr"/>
-      <c r="Y49" t="inlineStr"/>
+      <c r="X49" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z49" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento de placa receptora de condicionador de ar tipo split de 22.000 a 24.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5845,8 +6133,14 @@
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
-      <c r="X50" t="inlineStr"/>
-      <c r="Y50" t="inlineStr"/>
+      <c r="X50" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z50" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento de placa receptora de condicionador de ar tipo split de 30.000 a 36.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -5953,8 +6247,14 @@
       <c r="W51" t="n">
         <v>30.00597282365238</v>
       </c>
-      <c r="X51" t="inlineStr"/>
-      <c r="Y51" t="inlineStr"/>
+      <c r="X51" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z51" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento de placa receptora de condicionador de ar tipo split de 42.000 a 60.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6061,8 +6361,14 @@
       <c r="W52" t="n">
         <v>38.27795494290711</v>
       </c>
-      <c r="X52" t="inlineStr"/>
-      <c r="Y52" t="inlineStr"/>
+      <c r="X52" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z52" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da evaporadora de condicionador de ar tipo split de 7.000 a 10.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6169,8 +6475,14 @@
       <c r="W53" t="n">
         <v>30.01136567565951</v>
       </c>
-      <c r="X53" t="inlineStr"/>
-      <c r="Y53" t="inlineStr"/>
+      <c r="X53" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z53" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da evaporadora de condicionador de ar tipo split de 12.000 a 18.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6277,8 +6589,14 @@
       <c r="W54" t="n">
         <v>30.0021630975557</v>
       </c>
-      <c r="X54" t="inlineStr"/>
-      <c r="Y54" t="inlineStr"/>
+      <c r="X54" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z54" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da evaporadora de condicionador de ar tipo split de 22.000 a 24.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6385,8 +6703,14 @@
       <c r="W55" t="n">
         <v>29.8220741475863</v>
       </c>
-      <c r="X55" t="inlineStr"/>
-      <c r="Y55" t="inlineStr"/>
+      <c r="X55" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z55" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da evaporadora de condicionador de ar tipo split de 30.000 a 36.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6493,8 +6817,14 @@
       <c r="W56" t="n">
         <v>30.00349772647778</v>
       </c>
-      <c r="X56" t="inlineStr"/>
-      <c r="Y56" t="inlineStr"/>
+      <c r="X56" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z56" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da evaporadora de condicionador de ar tipo split de 42.000 a 60.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6601,8 +6931,14 @@
       <c r="W57" t="n">
         <v>34.15901487650367</v>
       </c>
-      <c r="X57" t="inlineStr"/>
-      <c r="Y57" t="inlineStr"/>
+      <c r="X57" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z57" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da condensadora de condicionador de ar tipo split de 7.000 a 10.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6709,8 +7045,14 @@
       <c r="W58" t="n">
         <v>29.35074226435342</v>
       </c>
-      <c r="X58" t="inlineStr"/>
-      <c r="Y58" t="inlineStr"/>
+      <c r="X58" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z58" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da condensadora de condicionador de ar tipo split de 12.000 a 18.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6817,8 +7159,14 @@
       <c r="W59" t="n">
         <v>29.99721003373323</v>
       </c>
-      <c r="X59" t="inlineStr"/>
-      <c r="Y59" t="inlineStr"/>
+      <c r="X59" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z59" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da condensadora de condicionador de ar tipo split de 22.000 a 24.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -6925,8 +7273,14 @@
       <c r="W60" t="n">
         <v>29.89104689720511</v>
       </c>
-      <c r="X60" t="inlineStr"/>
-      <c r="Y60" t="inlineStr"/>
+      <c r="X60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z60" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da condensadora de condicionador de ar tipo split de 30.000 a 36.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -7033,8 +7387,14 @@
       <c r="W61" t="n">
         <v>30.06993006993007</v>
       </c>
-      <c r="X61" t="inlineStr"/>
-      <c r="Y61" t="inlineStr"/>
+      <c r="X61" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z61" t="inlineStr">
         <is>
           <t>Serviço de manutenção corretiva com fornecimento e substituição de placa eletrônica da condensadora de condicionador de ar tipo split de 42.000 a 60.000 btu´s, de todos os modelos das marcas springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -7141,8 +7501,14 @@
       <c r="W62" t="n">
         <v>30.01918425223121</v>
       </c>
-      <c r="X62" t="inlineStr"/>
-      <c r="Y62" t="inlineStr"/>
+      <c r="X62" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z62" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 7.000 a 10.000 btu´s.</t>
@@ -7249,8 +7615,14 @@
       <c r="W63" t="n">
         <v>30.00446162998215</v>
       </c>
-      <c r="X63" t="inlineStr"/>
-      <c r="Y63" t="inlineStr"/>
+      <c r="X63" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z63" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 12.000 a 18.000 btu´s.</t>
@@ -7357,8 +7729,14 @@
       <c r="W64" t="n">
         <v>30.00381000762001</v>
       </c>
-      <c r="X64" t="inlineStr"/>
-      <c r="Y64" t="inlineStr"/>
+      <c r="X64" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z64" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 22.000 a 24.000 btu´s.</t>
@@ -7465,8 +7843,14 @@
       <c r="W65" t="n">
         <v>30.00171634532868</v>
       </c>
-      <c r="X65" t="inlineStr"/>
-      <c r="Y65" t="inlineStr"/>
+      <c r="X65" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y65" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z65" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 30.000 a 36.000 btu´s.</t>
@@ -7573,8 +7957,14 @@
       <c r="W66" t="n">
         <v>30.00306466441924</v>
       </c>
-      <c r="X66" t="inlineStr"/>
-      <c r="Y66" t="inlineStr"/>
+      <c r="X66" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y66" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z66" t="inlineStr">
         <is>
           <t>Serviço de manutenção preventiva com lavagem geral e lubrificação das condensadoras e evaporadoras de condicionadores de ar tipo split de 42.000 a 60.000 btu´s.</t>
@@ -7607,8 +7997,14 @@
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
       <c r="W67" t="inlineStr"/>
-      <c r="X67" t="inlineStr"/>
-      <c r="Y67" t="inlineStr"/>
+      <c r="X67" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z67" t="inlineStr">
         <is>
           <t>Serviço de manutençao corretiva com fornecimento e substituição de motoventilador da evaporadora de condicionador de ar tipo split de 7.000 a 10.000 btu´s, de todos os modelos da marca springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -7641,8 +8037,14 @@
       <c r="U68" t="inlineStr"/>
       <c r="V68" t="inlineStr"/>
       <c r="W68" t="inlineStr"/>
-      <c r="X68" t="inlineStr"/>
-      <c r="Y68" t="inlineStr"/>
+      <c r="X68" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z68" t="inlineStr">
         <is>
           <t>Serviço de manutençao corretiva com fornecimento e substituição de motoventilador da evaporadora de condicionador de ar tipo split de 12.000 a 18.000 btu´s, de todos os modelos da marca springer, midea, carrier, elgin, york, consul, lg, gree e eletrolux e komeco.</t>
@@ -7675,8 +8077,14 @@
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="inlineStr"/>
       <c r="W69" t="inlineStr"/>
-      <c r="X69" t="inlineStr"/>
-      <c r="Y69" t="inlineStr"/>
+      <c r="X69" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z69" t="inlineStr">
         <is>
           <t>IDEM AO ITEM 12 (ME/EPP)</t>
@@ -7709,8 +8117,14 @@
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr"/>
       <c r="W70" t="inlineStr"/>
-      <c r="X70" t="inlineStr"/>
-      <c r="Y70" t="inlineStr"/>
+      <c r="X70" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z70" t="inlineStr">
         <is>
           <t>IDEM AO ITEM 17 (ME/EPP)</t>

</xml_diff>